<commit_message>
primera tabla y referencias
</commit_message>
<xml_diff>
--- a/Docs/Resultados.xlsx
+++ b/Docs/Resultados.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oier\Documents\Uni\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oier\Desktop\TFG\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71056D70-F5F6-4A9A-946B-9009C2588277}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCE8DD9-B377-4FD4-A697-73A3E043A36C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{01D94149-3744-4B0D-BD6F-37A5A8AA1927}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{01D94149-3744-4B0D-BD6F-37A5A8AA1927}"/>
   </bookViews>
   <sheets>
     <sheet name="Rendimiento" sheetId="1" r:id="rId1"/>
+    <sheet name="Datasets" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>Iris</t>
   </si>
@@ -84,6 +85,72 @@
   </si>
   <si>
     <t>FARC-HD Local</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>#Atr.</t>
+  </si>
+  <si>
+    <t>iri</t>
+  </si>
+  <si>
+    <t>eco</t>
+  </si>
+  <si>
+    <t>pm</t>
+  </si>
+  <si>
+    <t>pima</t>
+  </si>
+  <si>
+    <t>yst</t>
+  </si>
+  <si>
+    <t>yeast</t>
+  </si>
+  <si>
+    <t>pag</t>
+  </si>
+  <si>
+    <t>pageblocks</t>
+  </si>
+  <si>
+    <t>ecoli</t>
+  </si>
+  <si>
+    <t>iris</t>
+  </si>
+  <si>
+    <t>wine</t>
+  </si>
+  <si>
+    <t>pen</t>
+  </si>
+  <si>
+    <t>penbased</t>
+  </si>
+  <si>
+    <t>mag</t>
+  </si>
+  <si>
+    <t>magic</t>
+  </si>
+  <si>
+    <t>clv</t>
+  </si>
+  <si>
+    <t>cleveland</t>
+  </si>
+  <si>
+    <t>#Clas.</t>
+  </si>
+  <si>
+    <t>#Ej.</t>
+  </si>
+  <si>
+    <t>id.</t>
   </si>
 </sst>
 </file>
@@ -272,66 +339,70 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,7 +719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A29AC6-A075-4882-9928-4C14C2F21FD5}">
   <dimension ref="B3:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -660,223 +731,218 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="24" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="24" t="s">
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
     </row>
     <row r="4" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="20"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="25" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="28"/>
-      <c r="I4" s="25" t="s">
+      <c r="H4" s="16"/>
+      <c r="I4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="J4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="K4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="15" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="16"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="10"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="6"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="3"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="6"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="3"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="6"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="3"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="6"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="3"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="6"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="3"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="6"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="3"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="6"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="3"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="9"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="6"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="13"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B3:C4"/>
@@ -885,8 +951,229 @@
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D329D1-F5AF-4CCB-A95A-B739CCF3B4D3}">
+  <dimension ref="A3:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="5.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="30">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="30">
+        <v>297</v>
+      </c>
+      <c r="E4" s="30">
+        <v>13</v>
+      </c>
+      <c r="F4" s="30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="30">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="30">
+        <v>336</v>
+      </c>
+      <c r="E5" s="30">
+        <v>7</v>
+      </c>
+      <c r="F5" s="30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="30">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="30">
+        <v>150</v>
+      </c>
+      <c r="E6" s="30">
+        <v>4</v>
+      </c>
+      <c r="F6" s="30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="30">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="30">
+        <v>19020</v>
+      </c>
+      <c r="E7" s="30">
+        <v>10</v>
+      </c>
+      <c r="F7" s="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="30">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="30">
+        <v>5472</v>
+      </c>
+      <c r="E8" s="30">
+        <v>10</v>
+      </c>
+      <c r="F8" s="30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="30">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="30">
+        <v>10992</v>
+      </c>
+      <c r="E9" s="30">
+        <v>16</v>
+      </c>
+      <c r="F9" s="30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="30">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="30">
+        <v>768</v>
+      </c>
+      <c r="E10" s="30">
+        <v>8</v>
+      </c>
+      <c r="F10" s="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="30">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="30">
+        <v>178</v>
+      </c>
+      <c r="E11" s="30">
+        <v>13</v>
+      </c>
+      <c r="F11" s="30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="30">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="30">
+        <v>1484</v>
+      </c>
+      <c r="E12" s="30">
+        <v>8</v>
+      </c>
+      <c r="F12" s="30">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>